<commit_message>
BCS/BCD generation scripts completed
</commit_message>
<xml_diff>
--- a/extdata/DS_OCADS_metadata_KAS.xlsx
+++ b/extdata/DS_OCADS_metadata_KAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogradye\Documents\Davis_Strait\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogradye\Documents\Davis_Strait\R_Working\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5181E8-55E5-43A7-B506-506D831884CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E51A49A-6A62-4A9A-AB5D-CE6716D71620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{23E6F023-7ED1-4C97-A670-340E58EBCB18}"/>
+    <workbookView xWindow="3570" yWindow="3570" windowWidth="21600" windowHeight="11280" xr2:uid="{23E6F023-7ED1-4C97-A670-340E58EBCB18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,18 +722,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44046919-837C-4920-B286-BC9DC9AA03D5}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.5703125" style="2" customWidth="1"/>
-    <col min="5" max="7" width="50.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="37.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="50.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1">
@@ -811,7 +811,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="150.75">
+    <row r="5" spans="1:7" ht="130.19999999999999">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -834,7 +834,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="270">
+    <row r="6" spans="1:7" ht="231">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -857,7 +857,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="150.75">
+    <row r="7" spans="1:7" ht="144.6">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -880,7 +880,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30.75">
+    <row r="8" spans="1:7" ht="29.4">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -972,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30.75">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -995,7 +995,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18">
+    <row r="13" spans="1:7" ht="17.399999999999999">
       <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18">
+    <row r="14" spans="1:7" ht="17.399999999999999">
       <c r="A14" s="13" t="s">
         <v>56</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18">
+    <row r="15" spans="1:7" ht="17.399999999999999">
       <c r="A15" s="13" t="s">
         <v>62</v>
       </c>
@@ -1061,10 +1061,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18">
+    <row r="16" spans="1:7" ht="17.399999999999999">
       <c r="A16" s="13"/>
     </row>
-    <row r="17" spans="1:1" ht="18">
+    <row r="17" spans="1:1" ht="17.399999999999999">
       <c r="A17" s="13"/>
     </row>
   </sheetData>

</xml_diff>